<commit_message>
create user ver 2.1
</commit_message>
<xml_diff>
--- a/ConnAutoTest.xlsx
+++ b/ConnAutoTest.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shehs\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shehs\PycharmProjects\pyTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F812F75-4DB6-4C6E-B99A-0DFB42F646CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92583BB0-1181-4A34-8AE5-86009B942359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="TestData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,43 +25,172 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>testing1</t>
-  </si>
-  <si>
-    <t>testing2</t>
-  </si>
-  <si>
-    <t>testing3</t>
-  </si>
-  <si>
-    <t>testing4</t>
-  </si>
-  <si>
-    <t>testing5</t>
-  </si>
-  <si>
-    <t>testing6</t>
-  </si>
-  <si>
-    <t>testing7</t>
-  </si>
-  <si>
-    <t>testing8</t>
-  </si>
-  <si>
-    <t>testing9</t>
-  </si>
-  <si>
-    <t>testing10</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
+  <si>
+    <t>Имя1</t>
+  </si>
+  <si>
+    <t>Имя2</t>
+  </si>
+  <si>
+    <t>Имя3</t>
+  </si>
+  <si>
+    <t>Имя4</t>
+  </si>
+  <si>
+    <t>Имя5</t>
+  </si>
+  <si>
+    <t>Имя6</t>
+  </si>
+  <si>
+    <t>Имя7</t>
+  </si>
+  <si>
+    <t>Имя8</t>
+  </si>
+  <si>
+    <t>Имя9</t>
+  </si>
+  <si>
+    <t>Имя10</t>
+  </si>
+  <si>
+    <t>Фамилияраз</t>
+  </si>
+  <si>
+    <t>Фамилиядва</t>
+  </si>
+  <si>
+    <t>Фамилиятри</t>
+  </si>
+  <si>
+    <t>Фамилиячетыре</t>
+  </si>
+  <si>
+    <t>Фамилияпять</t>
+  </si>
+  <si>
+    <t>Фамилияшесть</t>
+  </si>
+  <si>
+    <t>Фамилиясемь</t>
+  </si>
+  <si>
+    <t>Фамилиявосемь</t>
+  </si>
+  <si>
+    <t>Фамилиядевять</t>
+  </si>
+  <si>
+    <t>Фамилиядесять</t>
+  </si>
+  <si>
+    <t>Отчествораз</t>
+  </si>
+  <si>
+    <t>Отчестводва</t>
+  </si>
+  <si>
+    <t>Отчествотри</t>
+  </si>
+  <si>
+    <t>Отчествочетыре</t>
+  </si>
+  <si>
+    <t>Отчествопять</t>
+  </si>
+  <si>
+    <t>Отчествошесть</t>
+  </si>
+  <si>
+    <t>Отчествосемь</t>
+  </si>
+  <si>
+    <t>Отчествовосемь</t>
+  </si>
+  <si>
+    <t>Отчестводевять</t>
+  </si>
+  <si>
+    <t>Отчестводесять</t>
+  </si>
+  <si>
+    <t>pyTest1@gail.com</t>
+  </si>
+  <si>
+    <t>pyTest2@gail.com</t>
+  </si>
+  <si>
+    <t>pyTest3@gail.com</t>
+  </si>
+  <si>
+    <t>pyTest4@gail.com</t>
+  </si>
+  <si>
+    <t>pyTest5@gail.com</t>
+  </si>
+  <si>
+    <t>pyTest6@gail.com</t>
+  </si>
+  <si>
+    <t>pyTest7@gail.com</t>
+  </si>
+  <si>
+    <t>pyTest8@gail.com</t>
+  </si>
+  <si>
+    <t>pyTest9@gail.com</t>
+  </si>
+  <si>
+    <t>pyTest10@gail.com</t>
+  </si>
+  <si>
+    <t>Ментор</t>
+  </si>
+  <si>
+    <t>Продавец</t>
+  </si>
+  <si>
+    <t>Руководитель</t>
+  </si>
+  <si>
+    <t>Продавец-консультатнт</t>
+  </si>
+  <si>
+    <t>Фамилия</t>
+  </si>
+  <si>
+    <t>Имя</t>
+  </si>
+  <si>
+    <t>Отчество</t>
+  </si>
+  <si>
+    <t>Почта</t>
+  </si>
+  <si>
+    <t>Должность</t>
+  </si>
+  <si>
+    <t>Внутрений телефон</t>
+  </si>
+  <si>
+    <t>Моб.телефон</t>
+  </si>
+  <si>
+    <t>Кабинет</t>
+  </si>
+  <si>
+    <t>Дата рождения</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,6 +202,15 @@
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -96,8 +234,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -378,62 +518,340 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I2" sqref="I2:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2">
+        <v>69</v>
+      </c>
+      <c r="G2">
+        <v>89526541232</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2" s="1">
+        <v>34355</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3">
+        <v>123</v>
+      </c>
+      <c r="G3">
+        <v>84564561563</v>
+      </c>
+      <c r="H3">
+        <v>6</v>
+      </c>
+      <c r="I3" s="1">
+        <v>34356</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4">
+        <v>569</v>
+      </c>
+      <c r="G4">
+        <v>84581232356</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4" s="1">
+        <v>34357</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5">
+        <v>1254</v>
+      </c>
+      <c r="G5">
+        <v>84561238978</v>
+      </c>
+      <c r="H5">
+        <v>12</v>
+      </c>
+      <c r="I5" s="1">
+        <v>34358</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6">
+        <v>1235</v>
+      </c>
+      <c r="G6">
+        <v>89564567823</v>
+      </c>
+      <c r="H6">
+        <v>10</v>
+      </c>
+      <c r="I6" s="1">
+        <v>34359</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7">
+        <v>7895</v>
+      </c>
+      <c r="G7">
+        <v>89781263256</v>
+      </c>
+      <c r="H7">
+        <v>9</v>
+      </c>
+      <c r="I7" s="1">
+        <v>34360</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8">
+        <v>2589</v>
+      </c>
+      <c r="G8">
+        <v>87894562341</v>
+      </c>
+      <c r="H8">
+        <v>66</v>
+      </c>
+      <c r="I8" s="1">
+        <v>34361</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9">
+        <v>12547</v>
+      </c>
+      <c r="G9">
+        <v>84561237889</v>
+      </c>
+      <c r="H9">
+        <v>23</v>
+      </c>
+      <c r="I9" s="1">
+        <v>34362</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10">
+        <v>265</v>
+      </c>
+      <c r="G10">
+        <v>84569782345</v>
+      </c>
+      <c r="H10">
+        <v>145</v>
+      </c>
+      <c r="I10" s="1">
+        <v>34363</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
         <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11">
+        <v>23</v>
+      </c>
+      <c r="G11">
+        <v>89632021545</v>
+      </c>
+      <c r="H11">
+        <v>85</v>
+      </c>
+      <c r="I11" s="1">
+        <v>34364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>